<commit_message>
Added edit button for products on the list
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -561,8 +561,8 @@
   </sheetPr>
   <dimension ref="A1:I369"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A349" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H367" activeCellId="0" sqref="H367"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A202" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D219" activeCellId="0" sqref="D219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -6001,8 +6001,10 @@
       </c>
     </row>
     <row r="218" ht="15" customHeight="1" s="31">
-      <c r="A218" s="43" t="n">
-        <v>7898345393122</v>
+      <c r="A218" s="43" t="inlineStr">
+        <is>
+          <t>7898345393122</t>
+        </is>
       </c>
       <c r="B218" s="44" t="inlineStr">
         <is>
@@ -9816,7 +9818,7 @@
         </is>
       </c>
       <c r="D367" s="27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E367" s="27" t="n">
         <v>2</v>
@@ -9840,18 +9842,27 @@
           <t>090</t>
         </is>
       </c>
-      <c r="B368" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="C368" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="G368" t="n">
-        <v>23</v>
+      <c r="B368" s="26" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C368" s="26" t="inlineStr">
+        <is>
+          <t>rr</t>
+        </is>
+      </c>
+      <c r="D368" s="26" t="n">
+        <v>19</v>
+      </c>
+      <c r="E368" s="26" t="n">
+        <v>5</v>
+      </c>
+      <c r="F368" s="26" t="n">
+        <v>6</v>
+      </c>
+      <c r="G368" s="26" t="n">
+        <v>19</v>
       </c>
       <c r="H368" s="26" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
Made numlock always on
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -9872,7 +9872,30 @@
       </c>
     </row>
     <row r="369" ht="15" customHeight="1" s="31">
-      <c r="A369" s="26" t="n"/>
+      <c r="A369" s="26" t="inlineStr">
+        <is>
+          <t>99999</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>fsdfgsfg</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>4</v>
+      </c>
+      <c r="E369" t="n">
+        <v>4</v>
+      </c>
+      <c r="F369" t="n">
+        <v>3</v>
+      </c>
       <c r="G369" s="49" t="n"/>
       <c r="H369" s="26" t="n"/>
       <c r="I369" s="26" t="n"/>

</xml_diff>